<commit_message>
Unterschriften zu Protokollen hinzugefügt.
</commit_message>
<xml_diff>
--- a/protokolle/zeitaufzeichnung/krukenfellner.xlsx
+++ b/protokolle/zeitaufzeichnung/krukenfellner.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\juergen\repositories\SimpleQ\protokolle\zeitaufzeichnung\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{703E4209-A39D-40B2-8816-AE9328E957CB}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{439F715A-08E6-4A90-B9B4-B6E16809505B}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2775" yWindow="750" windowWidth="25365" windowHeight="14850" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Diplomprojekt" sheetId="1" r:id="rId1"/>
@@ -585,7 +585,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -715,6 +715,17 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -760,7 +771,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -798,20 +809,8 @@
     <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="20" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -819,6 +818,15 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="46" fontId="20" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
   </cellXfs>
@@ -1178,8 +1186,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C133"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H133" sqref="H133"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1190,10 +1198,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
+      <c r="B1" s="18"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -1249,1387 +1257,1387 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="19">
+      <c r="A8" s="15">
         <v>43295</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="20">
+      <c r="C8" s="16">
         <v>3.472222222222222E-3</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="19">
+      <c r="A9" s="15">
         <v>43296</v>
       </c>
-      <c r="B9" s="15" t="s">
+      <c r="B9" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="C9" s="20">
+      <c r="C9" s="16">
         <v>9.7222222222222224E-3</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="19">
+      <c r="A10" s="15">
         <v>43297</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C10" s="20">
+      <c r="C10" s="16">
         <v>5.9027777777777783E-2</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="19">
+      <c r="A11" s="15">
         <v>43298</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="13" t="s">
         <v>13</v>
       </c>
-      <c r="C11" s="20">
+      <c r="C11" s="16">
         <v>7.9166666666666663E-2</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="19">
+      <c r="A12" s="15">
         <v>43314</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="20">
+      <c r="C12" s="16">
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="19">
+      <c r="A13" s="15">
         <v>43334</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="20">
+      <c r="C13" s="16">
         <v>2.8472222222222222E-2</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="19">
+      <c r="A14" s="15">
         <v>43335</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C14" s="20">
+      <c r="C14" s="16">
         <v>7.7083333333333337E-2</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="19">
+      <c r="A15" s="15">
         <v>43337</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="20">
+      <c r="C15" s="16">
         <v>6.6666666666666666E-2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="19">
+      <c r="A16" s="15">
         <v>43338</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C16" s="20">
+      <c r="C16" s="16">
         <v>2.7777777777777776E-2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="19">
+      <c r="A17" s="15">
         <v>43340</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="20">
+      <c r="C17" s="16">
         <v>6.3194444444444442E-2</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="19">
+      <c r="A18" s="15">
         <v>43340</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C18" s="20">
+      <c r="C18" s="16">
         <v>4.027777777777778E-2</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="19">
+      <c r="A19" s="15">
         <v>43341</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C19" s="20">
+      <c r="C19" s="16">
         <v>8.7500000000000008E-2</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="19">
+      <c r="A20" s="15">
         <v>43342</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="20">
+      <c r="C20" s="16">
         <v>2.4305555555555556E-2</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="19">
+      <c r="A21" s="15">
         <v>43344</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="20">
+      <c r="C21" s="16">
         <v>1.3888888888888888E-2</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="19">
+      <c r="A22" s="15">
         <v>43345</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C22" s="20">
+      <c r="C22" s="16">
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="19">
+      <c r="A23" s="15">
         <v>43346</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="C23" s="20">
+      <c r="C23" s="16">
         <v>8.1250000000000003E-2</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="19">
+      <c r="A24" s="15">
         <v>43347</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C24" s="20">
+      <c r="C24" s="16">
         <v>5.2083333333333336E-2</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="19">
+      <c r="A25" s="15">
         <v>43349</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C25" s="20">
+      <c r="C25" s="16">
         <v>2.1527777777777781E-2</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="19">
+      <c r="A26" s="15">
         <v>43350</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C26" s="20">
+      <c r="C26" s="16">
         <v>6.0416666666666667E-2</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="19">
+      <c r="A27" s="15">
         <v>43352</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C27" s="20">
+      <c r="C27" s="16">
         <v>6.9444444444444441E-3</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="19">
+      <c r="A28" s="15">
         <v>43353</v>
       </c>
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C28" s="20">
+      <c r="C28" s="16">
         <v>1.6666666666666666E-2</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="19">
+      <c r="A29" s="15">
         <v>43354</v>
       </c>
-      <c r="B29" s="14" t="s">
+      <c r="B29" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C29" s="20">
+      <c r="C29" s="16">
         <v>0.21736111111111112</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="19">
+      <c r="A30" s="15">
         <v>43355</v>
       </c>
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C30" s="20">
+      <c r="C30" s="16">
         <v>4.7916666666666663E-2</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="19">
+      <c r="A31" s="15">
         <v>43356</v>
       </c>
-      <c r="B31" s="14" t="s">
+      <c r="B31" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C31" s="20">
+      <c r="C31" s="16">
         <v>0.12152777777777778</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="19">
+      <c r="A32" s="15">
         <v>43357</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="C32" s="20">
+      <c r="C32" s="16">
         <v>1.3888888888888888E-2</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="19">
+      <c r="A33" s="15">
         <v>43358</v>
       </c>
-      <c r="B33" s="14" t="s">
+      <c r="B33" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C33" s="20">
+      <c r="C33" s="16">
         <v>1.5972222222222224E-2</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="19">
+      <c r="A34" s="15">
         <v>43359</v>
       </c>
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C34" s="20">
+      <c r="C34" s="16">
         <v>6.3194444444444442E-2</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="19">
+      <c r="A35" s="15">
         <v>43359</v>
       </c>
-      <c r="B35" s="14" t="s">
+      <c r="B35" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C35" s="20">
+      <c r="C35" s="16">
         <v>1.3888888888888888E-2</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="19">
+      <c r="A36" s="15">
         <v>43360</v>
       </c>
-      <c r="B36" s="14" t="s">
+      <c r="B36" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C36" s="20">
+      <c r="C36" s="16">
         <v>8.1250000000000003E-2</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="19">
+      <c r="A37" s="15">
         <v>43361</v>
       </c>
-      <c r="B37" s="14" t="s">
+      <c r="B37" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C37" s="20">
+      <c r="C37" s="16">
         <v>0.1388888888888889</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="19">
+      <c r="A38" s="15">
         <v>43362</v>
       </c>
-      <c r="B38" s="14" t="s">
+      <c r="B38" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C38" s="20">
+      <c r="C38" s="16">
         <v>0.11388888888888889</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="19">
+      <c r="A39" s="15">
         <v>43363</v>
       </c>
-      <c r="B39" s="14" t="s">
+      <c r="B39" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C39" s="20">
+      <c r="C39" s="16">
         <v>4.4444444444444446E-2</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="19">
+      <c r="A40" s="15">
         <v>43366</v>
       </c>
-      <c r="B40" s="14" t="s">
+      <c r="B40" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C40" s="20">
+      <c r="C40" s="16">
         <v>5.347222222222222E-2</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="19">
+      <c r="A41" s="15">
         <v>43367</v>
       </c>
-      <c r="B41" s="14" t="s">
+      <c r="B41" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C41" s="20">
+      <c r="C41" s="16">
         <v>9.9999999999999992E-2</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="19">
+      <c r="A42" s="15">
         <v>43368</v>
       </c>
-      <c r="B42" s="14" t="s">
+      <c r="B42" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C42" s="20">
+      <c r="C42" s="16">
         <v>0.20138888888888887</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="19">
+      <c r="A43" s="15">
         <v>43370</v>
       </c>
-      <c r="B43" s="14" t="s">
+      <c r="B43" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C43" s="20">
+      <c r="C43" s="16">
         <v>9.0972222222222218E-2</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A44" s="19">
+      <c r="A44" s="15">
         <v>43371</v>
       </c>
-      <c r="B44" s="14" t="s">
+      <c r="B44" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C44" s="20">
+      <c r="C44" s="16">
         <v>8.819444444444445E-2</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="19">
+      <c r="A45" s="15">
         <v>43371</v>
       </c>
-      <c r="B45" s="14" t="s">
+      <c r="B45" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C45" s="20">
+      <c r="C45" s="16">
         <v>2.7083333333333334E-2</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="19">
+      <c r="A46" s="15">
         <v>43372</v>
       </c>
-      <c r="B46" s="14" t="s">
+      <c r="B46" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C46" s="20">
+      <c r="C46" s="16">
         <v>5.9027777777777783E-2</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="19">
+      <c r="A47" s="15">
         <v>43373</v>
       </c>
-      <c r="B47" s="14" t="s">
+      <c r="B47" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C47" s="20">
+      <c r="C47" s="16">
         <v>4.4444444444444446E-2</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="19">
+      <c r="A48" s="15">
         <v>43374</v>
       </c>
-      <c r="B48" s="14" t="s">
+      <c r="B48" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C48" s="20">
+      <c r="C48" s="16">
         <v>2.5694444444444447E-2</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="19">
+      <c r="A49" s="15">
         <v>43375</v>
       </c>
-      <c r="B49" s="14" t="s">
+      <c r="B49" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C49" s="20">
+      <c r="C49" s="16">
         <v>0.16111111111111112</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A50" s="19">
+      <c r="A50" s="15">
         <v>43377</v>
       </c>
-      <c r="B50" s="14" t="s">
+      <c r="B50" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="C50" s="20">
+      <c r="C50" s="16">
         <v>6.3194444444444442E-2</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="19">
+      <c r="A51" s="15">
         <v>43378</v>
       </c>
-      <c r="B51" s="14" t="s">
+      <c r="B51" s="13" t="s">
         <v>17</v>
       </c>
-      <c r="C51" s="20">
+      <c r="C51" s="16">
         <v>4.5138888888888888E-2</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A52" s="19">
+      <c r="A52" s="15">
         <v>43381</v>
       </c>
-      <c r="B52" s="14" t="s">
+      <c r="B52" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C52" s="20">
+      <c r="C52" s="16">
         <v>4.0972222222222222E-2</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="19">
+      <c r="A53" s="15">
         <v>43382</v>
       </c>
-      <c r="B53" s="14" t="s">
+      <c r="B53" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C53" s="20">
+      <c r="C53" s="16">
         <v>0.22569444444444445</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A54" s="19">
+      <c r="A54" s="15">
         <v>43383</v>
       </c>
-      <c r="B54" s="14" t="s">
+      <c r="B54" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C54" s="20">
+      <c r="C54" s="16">
         <v>1.8749999999999999E-2</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="19">
+      <c r="A55" s="15">
         <v>43385</v>
       </c>
-      <c r="B55" s="14" t="s">
+      <c r="B55" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C55" s="20">
+      <c r="C55" s="16">
         <v>6.3194444444444442E-2</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A56" s="19">
+      <c r="A56" s="15">
         <v>43386</v>
       </c>
-      <c r="B56" s="14" t="s">
+      <c r="B56" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C56" s="20">
+      <c r="C56" s="16">
         <v>8.3333333333333329E-2</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A57" s="19">
+      <c r="A57" s="15">
         <v>43386</v>
       </c>
-      <c r="B57" s="14" t="s">
+      <c r="B57" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C57" s="20">
+      <c r="C57" s="16">
         <v>4.8611111111111112E-2</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A58" s="19">
+      <c r="A58" s="15">
         <v>43389</v>
       </c>
-      <c r="B58" s="14" t="s">
+      <c r="B58" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C58" s="20">
+      <c r="C58" s="16">
         <v>0.16319444444444445</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A59" s="19">
+      <c r="A59" s="15">
         <v>43391</v>
       </c>
-      <c r="B59" s="14" t="s">
+      <c r="B59" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="C59" s="20">
+      <c r="C59" s="16">
         <v>2.4999999999999998E-2</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A60" s="19">
+      <c r="A60" s="15">
         <v>43396</v>
       </c>
-      <c r="B60" s="14" t="s">
+      <c r="B60" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C60" s="20">
+      <c r="C60" s="16">
         <v>0.26874999999999999</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A61" s="19">
+      <c r="A61" s="15">
         <v>43396</v>
       </c>
-      <c r="B61" s="14" t="s">
+      <c r="B61" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C61" s="20">
+      <c r="C61" s="16">
         <v>6.5277777777777782E-2</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A62" s="19">
+      <c r="A62" s="15">
         <v>43398</v>
       </c>
-      <c r="B62" s="14" t="s">
+      <c r="B62" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C62" s="20">
+      <c r="C62" s="16">
         <v>4.3055555555555562E-2</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A63" s="19">
+      <c r="A63" s="15">
         <v>43402</v>
       </c>
-      <c r="B63" s="14" t="s">
+      <c r="B63" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C63" s="20">
+      <c r="C63" s="16">
         <v>0.11527777777777777</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A64" s="19">
+      <c r="A64" s="15">
         <v>43408</v>
       </c>
-      <c r="B64" s="14" t="s">
+      <c r="B64" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C64" s="20">
+      <c r="C64" s="16">
         <v>4.7222222222222221E-2</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A65" s="19">
+      <c r="A65" s="15">
         <v>43409</v>
       </c>
-      <c r="B65" s="14" t="s">
+      <c r="B65" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C65" s="20">
+      <c r="C65" s="16">
         <v>9.0972222222222218E-2</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="19">
+      <c r="A66" s="15">
         <v>43410</v>
       </c>
-      <c r="B66" s="14" t="s">
+      <c r="B66" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C66" s="20">
+      <c r="C66" s="16">
         <v>0.19513888888888889</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="19">
+      <c r="A67" s="15">
         <v>43411</v>
       </c>
-      <c r="B67" s="14" t="s">
+      <c r="B67" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C67" s="20">
+      <c r="C67" s="16">
         <v>7.3611111111111113E-2</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="19">
+      <c r="A68" s="15">
         <v>43412</v>
       </c>
-      <c r="B68" s="14" t="s">
+      <c r="B68" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C68" s="20">
+      <c r="C68" s="16">
         <v>6.0416666666666667E-2</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="19">
+      <c r="A69" s="15">
         <v>43417</v>
       </c>
-      <c r="B69" s="14" t="s">
+      <c r="B69" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C69" s="20">
+      <c r="C69" s="16">
         <v>0.11041666666666666</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="19">
+      <c r="A70" s="15">
         <v>43418</v>
       </c>
-      <c r="B70" s="14" t="s">
+      <c r="B70" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C70" s="20">
+      <c r="C70" s="16">
         <v>2.9861111111111113E-2</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A71" s="19">
+      <c r="A71" s="15">
         <v>43419</v>
       </c>
-      <c r="B71" s="14" t="s">
+      <c r="B71" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C71" s="20">
+      <c r="C71" s="16">
         <v>3.9583333333333331E-2</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A72" s="19">
+      <c r="A72" s="15">
         <v>43420</v>
       </c>
-      <c r="B72" s="14" t="s">
+      <c r="B72" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C72" s="20">
+      <c r="C72" s="16">
         <v>8.4027777777777771E-2</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="19">
+      <c r="A73" s="15">
         <v>43422</v>
       </c>
-      <c r="B73" s="14" t="s">
+      <c r="B73" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C73" s="20">
+      <c r="C73" s="16">
         <v>0.11180555555555556</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="19">
+      <c r="A74" s="15">
         <v>43422</v>
       </c>
-      <c r="B74" s="14" t="s">
+      <c r="B74" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="C74" s="20">
+      <c r="C74" s="16">
         <v>6.2499999999999995E-3</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="19">
+      <c r="A75" s="15">
         <v>43424</v>
       </c>
-      <c r="B75" s="14" t="s">
+      <c r="B75" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C75" s="20">
+      <c r="C75" s="16">
         <v>0.18958333333333333</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="19">
+      <c r="A76" s="15">
         <v>43425</v>
       </c>
-      <c r="B76" s="14" t="s">
+      <c r="B76" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C76" s="20">
+      <c r="C76" s="16">
         <v>0.13194444444444445</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A77" s="19">
+      <c r="A77" s="15">
         <v>43425</v>
       </c>
-      <c r="B77" s="14" t="s">
+      <c r="B77" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C77" s="20">
+      <c r="C77" s="16">
         <v>3.8194444444444441E-2</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A78" s="19">
+      <c r="A78" s="15">
         <v>43425</v>
       </c>
-      <c r="B78" s="14" t="s">
+      <c r="B78" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C78" s="20">
+      <c r="C78" s="16">
         <v>2.9861111111111113E-2</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A79" s="19">
+      <c r="A79" s="15">
         <v>43426</v>
       </c>
-      <c r="B79" s="14" t="s">
+      <c r="B79" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="C79" s="20">
+      <c r="C79" s="16">
         <v>2.7083333333333334E-2</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A80" s="19">
+      <c r="A80" s="15">
         <v>43430</v>
       </c>
-      <c r="B80" s="14" t="s">
+      <c r="B80" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C80" s="20">
+      <c r="C80" s="16">
         <v>9.0972222222222218E-2</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="19">
+      <c r="A81" s="15">
         <v>43431</v>
       </c>
-      <c r="B81" s="14" t="s">
+      <c r="B81" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="C81" s="20">
+      <c r="C81" s="16">
         <v>0.22916666666666666</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="19">
+      <c r="A82" s="15">
         <v>43432</v>
       </c>
-      <c r="B82" s="14" t="s">
+      <c r="B82" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C82" s="20">
+      <c r="C82" s="16">
         <v>0.10625</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A83" s="19">
+      <c r="A83" s="15">
         <v>43433</v>
       </c>
-      <c r="B83" s="14" t="s">
+      <c r="B83" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C83" s="20">
+      <c r="C83" s="16">
         <v>6.25E-2</v>
       </c>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A84" s="19">
+      <c r="A84" s="15">
         <v>43435</v>
       </c>
-      <c r="B84" s="14" t="s">
+      <c r="B84" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C84" s="20">
+      <c r="C84" s="16">
         <v>5.4166666666666669E-2</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A85" s="19">
+      <c r="A85" s="15">
         <v>43436</v>
       </c>
-      <c r="B85" s="14" t="s">
+      <c r="B85" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C85" s="20">
+      <c r="C85" s="16">
         <v>0.16597222222222222</v>
       </c>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A86" s="19">
+      <c r="A86" s="15">
         <v>43437</v>
       </c>
-      <c r="B86" s="14" t="s">
+      <c r="B86" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="C86" s="20">
+      <c r="C86" s="16">
         <v>6.9444444444444434E-2</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A87" s="19">
+      <c r="A87" s="15">
         <v>43438</v>
       </c>
-      <c r="B87" s="14" t="s">
+      <c r="B87" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C87" s="20">
+      <c r="C87" s="16">
         <v>0.21597222222222223</v>
       </c>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A88" s="19">
+      <c r="A88" s="15">
         <v>43439</v>
       </c>
-      <c r="B88" s="14" t="s">
+      <c r="B88" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C88" s="20">
+      <c r="C88" s="16">
         <v>5.2777777777777778E-2</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A89" s="19">
+      <c r="A89" s="15">
         <v>43440</v>
       </c>
-      <c r="B89" s="14" t="s">
+      <c r="B89" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C89" s="20">
+      <c r="C89" s="16">
         <v>0.11875000000000001</v>
       </c>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A90" s="19">
+      <c r="A90" s="15">
         <v>43442</v>
       </c>
-      <c r="B90" s="14" t="s">
+      <c r="B90" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="C90" s="20">
+      <c r="C90" s="16">
         <v>5.2777777777777778E-2</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A91" s="19">
+      <c r="A91" s="15">
         <v>43443</v>
       </c>
-      <c r="B91" s="14" t="s">
+      <c r="B91" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C91" s="20">
+      <c r="C91" s="16">
         <v>9.8611111111111108E-2</v>
       </c>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A92" s="19">
+      <c r="A92" s="15">
         <v>43445</v>
       </c>
-      <c r="B92" s="14" t="s">
+      <c r="B92" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C92" s="20">
+      <c r="C92" s="16">
         <v>0.21041666666666667</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A93" s="19">
+      <c r="A93" s="15">
         <v>43445</v>
       </c>
-      <c r="B93" s="14" t="s">
+      <c r="B93" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="C93" s="20">
+      <c r="C93" s="16">
         <v>1.2499999999999999E-2</v>
       </c>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A94" s="19">
+      <c r="A94" s="15">
         <v>43446</v>
       </c>
-      <c r="B94" s="14" t="s">
+      <c r="B94" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C94" s="20">
+      <c r="C94" s="16">
         <v>1.5277777777777777E-2</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A95" s="19">
+      <c r="A95" s="15">
         <v>43448</v>
       </c>
-      <c r="B95" s="14" t="s">
+      <c r="B95" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="C95" s="20">
+      <c r="C95" s="16">
         <v>9.7222222222222224E-3</v>
       </c>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A96" s="19">
+      <c r="A96" s="15">
         <v>43452</v>
       </c>
-      <c r="B96" s="14" t="s">
+      <c r="B96" s="13" t="s">
         <v>34</v>
       </c>
-      <c r="C96" s="20">
+      <c r="C96" s="16">
         <v>0.17361111111111113</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A97" s="19">
+      <c r="A97" s="15">
         <v>43452</v>
       </c>
-      <c r="B97" s="14" t="s">
+      <c r="B97" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="C97" s="20">
+      <c r="C97" s="16">
         <v>6.2499999999999995E-3</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A98" s="19">
+      <c r="A98" s="15">
         <v>43454</v>
       </c>
-      <c r="B98" s="14" t="s">
+      <c r="B98" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="C98" s="20">
+      <c r="C98" s="16">
         <v>7.6388888888888886E-3</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A99" s="19">
+      <c r="A99" s="15">
         <v>43455</v>
       </c>
-      <c r="B99" s="14" t="s">
+      <c r="B99" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="C99" s="20">
+      <c r="C99" s="16">
         <v>0.12013888888888889</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A100" s="19">
+      <c r="A100" s="15">
         <v>43455</v>
       </c>
-      <c r="B100" s="14" t="s">
+      <c r="B100" s="13" t="s">
         <v>35</v>
       </c>
-      <c r="C100" s="20">
+      <c r="C100" s="16">
         <v>2.2916666666666669E-2</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A101" s="19">
+      <c r="A101" s="15">
         <v>43473</v>
       </c>
-      <c r="B101" s="14" t="s">
+      <c r="B101" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C101" s="20">
+      <c r="C101" s="16">
         <v>0.13819444444444443</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A102" s="19">
+      <c r="A102" s="15">
         <v>43473</v>
       </c>
-      <c r="B102" s="14" t="s">
+      <c r="B102" s="13" t="s">
         <v>37</v>
       </c>
-      <c r="C102" s="20">
+      <c r="C102" s="16">
         <v>6.1805555555555558E-2</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A103" s="19">
+      <c r="A103" s="15">
         <v>43474</v>
       </c>
-      <c r="B103" s="14" t="s">
+      <c r="B103" s="13" t="s">
         <v>38</v>
       </c>
-      <c r="C103" s="20">
+      <c r="C103" s="16">
         <v>0.10694444444444444</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A104" s="19">
+      <c r="A104" s="15">
         <v>43474</v>
       </c>
-      <c r="B104" s="14" t="s">
+      <c r="B104" s="13" t="s">
         <v>36</v>
       </c>
-      <c r="C104" s="20">
+      <c r="C104" s="16">
         <v>2.6388888888888889E-2</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A105" s="19">
+      <c r="A105" s="15">
         <v>43475</v>
       </c>
-      <c r="B105" s="14" t="s">
+      <c r="B105" s="13" t="s">
         <v>39</v>
       </c>
-      <c r="C105" s="20">
+      <c r="C105" s="16">
         <v>0.18333333333333335</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A106" s="19">
+      <c r="A106" s="15">
         <v>43476</v>
       </c>
-      <c r="B106" s="14" t="s">
+      <c r="B106" s="13" t="s">
         <v>40</v>
       </c>
-      <c r="C106" s="20">
+      <c r="C106" s="16">
         <v>4.2361111111111106E-2</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A107" s="19">
+      <c r="A107" s="15">
         <v>43476</v>
       </c>
-      <c r="B107" s="14" t="s">
+      <c r="B107" s="13" t="s">
         <v>41</v>
       </c>
-      <c r="C107" s="20">
+      <c r="C107" s="16">
         <v>2.361111111111111E-2</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A108" s="19">
+      <c r="A108" s="15">
         <v>43480</v>
       </c>
-      <c r="B108" s="14" t="s">
+      <c r="B108" s="13" t="s">
         <v>42</v>
       </c>
-      <c r="C108" s="20">
+      <c r="C108" s="16">
         <v>6.458333333333334E-2</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A109" s="19">
+      <c r="A109" s="15">
         <v>43480</v>
       </c>
-      <c r="B109" s="14" t="s">
+      <c r="B109" s="13" t="s">
         <v>43</v>
       </c>
-      <c r="C109" s="20">
+      <c r="C109" s="16">
         <v>6.1805555555555558E-2</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A110" s="19">
+      <c r="A110" s="15">
         <v>43482</v>
       </c>
-      <c r="B110" s="14" t="s">
+      <c r="B110" s="13" t="s">
         <v>44</v>
       </c>
-      <c r="C110" s="20">
+      <c r="C110" s="16">
         <v>6.5277777777777782E-2</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A111" s="19">
+      <c r="A111" s="15">
         <v>43493</v>
       </c>
-      <c r="B111" s="14" t="s">
+      <c r="B111" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C111" s="20">
+      <c r="C111" s="16">
         <v>9.2361111111111116E-2</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A112" s="19">
+      <c r="A112" s="15">
         <v>43493</v>
       </c>
-      <c r="B112" s="14" t="s">
+      <c r="B112" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="C112" s="20">
+      <c r="C112" s="16">
         <v>5.0694444444444452E-2</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A113" s="19">
+      <c r="A113" s="15">
         <v>43494</v>
       </c>
-      <c r="B113" s="14" t="s">
+      <c r="B113" s="13" t="s">
         <v>45</v>
       </c>
-      <c r="C113" s="20">
+      <c r="C113" s="16">
         <v>4.2361111111111106E-2</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A114" s="19">
+      <c r="A114" s="15">
         <v>43495</v>
       </c>
-      <c r="B114" s="14" t="s">
+      <c r="B114" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C114" s="20">
+      <c r="C114" s="16">
         <v>2.6388888888888889E-2</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A115" s="19">
+      <c r="A115" s="15">
         <v>43508</v>
       </c>
-      <c r="B115" s="14" t="s">
+      <c r="B115" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C115" s="20">
+      <c r="C115" s="16">
         <v>0.31319444444444444</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A116" s="19">
+      <c r="A116" s="15">
         <v>43509</v>
       </c>
-      <c r="B116" s="14" t="s">
+      <c r="B116" s="13" t="s">
         <v>48</v>
       </c>
-      <c r="C116" s="20">
+      <c r="C116" s="16">
         <v>0.11875000000000001</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A117" s="19">
+      <c r="A117" s="15">
         <v>43509</v>
       </c>
-      <c r="B117" s="14" t="s">
+      <c r="B117" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C117" s="20">
+      <c r="C117" s="16">
         <v>7.013888888888889E-2</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A118" s="19">
+      <c r="A118" s="15">
         <v>43515</v>
       </c>
-      <c r="B118" s="14" t="s">
+      <c r="B118" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="C118" s="20">
+      <c r="C118" s="16">
         <v>6.1805555555555558E-2</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A119" s="19">
+      <c r="A119" s="15">
         <v>43518</v>
       </c>
-      <c r="B119" s="14" t="s">
+      <c r="B119" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="C119" s="20">
+      <c r="C119" s="16">
         <v>3.3333333333333333E-2</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A120" s="19">
+      <c r="A120" s="15">
         <v>43522</v>
       </c>
-      <c r="B120" s="14" t="s">
+      <c r="B120" s="13" t="s">
         <v>47</v>
       </c>
-      <c r="C120" s="20">
+      <c r="C120" s="16">
         <v>6.6666666666666666E-2</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A121" s="19">
+      <c r="A121" s="15">
         <v>43524</v>
       </c>
-      <c r="B121" s="14" t="s">
+      <c r="B121" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="C121" s="20">
+      <c r="C121" s="16">
         <v>7.9166666666666663E-2</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A122" s="19">
+      <c r="A122" s="15">
         <v>43524</v>
       </c>
-      <c r="B122" s="14" t="s">
+      <c r="B122" s="13" t="s">
         <v>52</v>
       </c>
-      <c r="C122" s="20">
+      <c r="C122" s="16">
         <v>2.2222222222222223E-2</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A123" s="19">
+      <c r="A123" s="15">
         <v>43525</v>
       </c>
-      <c r="B123" s="14" t="s">
+      <c r="B123" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="C123" s="20">
+      <c r="C123" s="16">
         <v>0.18541666666666667</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A124" s="19">
+      <c r="A124" s="15">
         <v>43526</v>
       </c>
-      <c r="B124" s="14" t="s">
+      <c r="B124" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="C124" s="20">
+      <c r="C124" s="16">
         <v>8.5416666666666655E-2</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A125" s="19">
+      <c r="A125" s="15">
         <v>43527</v>
       </c>
-      <c r="B125" s="14" t="s">
+      <c r="B125" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="C125" s="20">
+      <c r="C125" s="16">
         <v>2.4999999999999998E-2</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A126" s="19">
+      <c r="A126" s="15">
         <v>43527</v>
       </c>
-      <c r="B126" s="14" t="s">
+      <c r="B126" s="13" t="s">
         <v>55</v>
       </c>
-      <c r="C126" s="20">
+      <c r="C126" s="16">
         <v>2.013888888888889E-2</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A127" s="19">
+      <c r="A127" s="15">
         <v>43528</v>
       </c>
-      <c r="B127" s="14" t="s">
+      <c r="B127" s="13" t="s">
         <v>54</v>
       </c>
-      <c r="C127" s="20">
+      <c r="C127" s="16">
         <v>2.0833333333333332E-2</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A128" s="19">
+      <c r="A128" s="15">
         <v>43529</v>
       </c>
-      <c r="B128" s="14" t="s">
+      <c r="B128" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="C128" s="20">
+      <c r="C128" s="16">
         <v>0.14583333333333334</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A129" s="19">
+      <c r="A129" s="15">
         <v>43529</v>
       </c>
-      <c r="B129" s="14" t="s">
+      <c r="B129" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="C129" s="20">
+      <c r="C129" s="16">
         <v>7.4305555555555555E-2</v>
       </c>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A130" s="19">
+      <c r="A130" s="15">
         <v>43530</v>
       </c>
-      <c r="B130" s="14" t="s">
+      <c r="B130" s="13" t="s">
         <v>57</v>
       </c>
-      <c r="C130" s="20">
+      <c r="C130" s="16">
         <v>8.3333333333333332E-3</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A131" s="19">
+      <c r="A131" s="15">
         <v>43535</v>
       </c>
-      <c r="B131" s="14" t="s">
+      <c r="B131" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="C131" s="20">
+      <c r="C131" s="16">
         <v>3.1944444444444449E-2</v>
       </c>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A132" s="19">
+      <c r="A132" s="15">
         <v>43542</v>
       </c>
-      <c r="B132" s="14" t="s">
+      <c r="B132" s="13" t="s">
         <v>58</v>
       </c>
-      <c r="C132" s="20">
+      <c r="C132" s="16">
         <f>SUM(C8:C131)</f>
         <v>9.3645833333333375</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A133" s="4"/>
-      <c r="B133" s="16" t="s">
+      <c r="A133" s="20"/>
+      <c r="B133" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C133" s="21">
+      <c r="C133" s="17">
         <f>SUM(C132)</f>
         <v>9.3645833333333375</v>
       </c>
@@ -2647,8 +2655,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="E38" sqref="E38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2659,10 +2667,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="26.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="18" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="13"/>
+      <c r="B1" s="18"/>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
@@ -2718,341 +2726,341 @@
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="19">
+      <c r="A8" s="15">
         <v>43392</v>
       </c>
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="13" t="s">
         <v>59</v>
       </c>
-      <c r="C8" s="20">
+      <c r="C8" s="16">
         <v>1.0416666666666666E-2</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="19">
+      <c r="A9" s="15">
         <v>43401</v>
       </c>
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="20">
+      <c r="C9" s="16">
         <v>8.5416666666666655E-2</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="19">
+      <c r="A10" s="15">
         <v>43402</v>
       </c>
-      <c r="B10" s="14" t="s">
+      <c r="B10" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="C10" s="20">
+      <c r="C10" s="16">
         <v>2.8472222222222222E-2</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="19">
+      <c r="A11" s="15">
         <v>43403</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="C11" s="20">
+      <c r="C11" s="16">
         <v>1.5972222222222224E-2</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="19">
+      <c r="A12" s="15">
         <v>43422</v>
       </c>
-      <c r="B12" s="14" t="s">
+      <c r="B12" s="13" t="s">
         <v>60</v>
       </c>
-      <c r="C12" s="20">
+      <c r="C12" s="16">
         <v>3.4722222222222224E-2</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="19">
+      <c r="A13" s="15">
         <v>43463</v>
       </c>
-      <c r="B13" s="14" t="s">
+      <c r="B13" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="C13" s="20">
+      <c r="C13" s="16">
         <v>7.7777777777777779E-2</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A14" s="19">
+      <c r="A14" s="15">
         <v>43464</v>
       </c>
-      <c r="B14" s="14" t="s">
+      <c r="B14" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="C14" s="20">
+      <c r="C14" s="16">
         <v>9.1666666666666674E-2</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" s="19">
+      <c r="A15" s="15">
         <v>43465</v>
       </c>
-      <c r="B15" s="14" t="s">
+      <c r="B15" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="C15" s="20">
+      <c r="C15" s="16">
         <v>3.9583333333333331E-2</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="19">
+      <c r="A16" s="15">
         <v>43467</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="B16" s="13" t="s">
         <v>62</v>
       </c>
-      <c r="C16" s="20">
+      <c r="C16" s="16">
         <v>5.2777777777777778E-2</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" s="19">
+      <c r="A17" s="15">
         <v>43468</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="B17" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="C17" s="20">
+      <c r="C17" s="16">
         <v>7.9861111111111105E-2</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" s="19">
+      <c r="A18" s="15">
         <v>43495</v>
       </c>
-      <c r="B18" s="14" t="s">
+      <c r="B18" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="C18" s="20">
+      <c r="C18" s="16">
         <v>1.3888888888888888E-2</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" s="19">
+      <c r="A19" s="15">
         <v>43499</v>
       </c>
-      <c r="B19" s="14" t="s">
+      <c r="B19" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="C19" s="20">
+      <c r="C19" s="16">
         <v>4.3055555555555562E-2</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" s="19">
+      <c r="A20" s="15">
         <v>43500</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="C20" s="20">
+      <c r="C20" s="16">
         <v>5.486111111111111E-2</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" s="19">
+      <c r="A21" s="15">
         <v>43500</v>
       </c>
-      <c r="B21" s="14" t="s">
+      <c r="B21" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="C21" s="20">
+      <c r="C21" s="16">
         <v>6.9444444444444441E-3</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" s="19">
+      <c r="A22" s="15">
         <v>43501</v>
       </c>
-      <c r="B22" s="14" t="s">
+      <c r="B22" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C22" s="20">
+      <c r="C22" s="16">
         <v>7.9166666666666663E-2</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" s="19">
+      <c r="A23" s="15">
         <v>43502</v>
       </c>
-      <c r="B23" s="14" t="s">
+      <c r="B23" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="C23" s="20">
+      <c r="C23" s="16">
         <v>5.8333333333333327E-2</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" s="19">
+      <c r="A24" s="15">
         <v>43503</v>
       </c>
-      <c r="B24" s="14" t="s">
+      <c r="B24" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="C24" s="20">
+      <c r="C24" s="16">
         <v>5.5555555555555552E-2</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" s="19">
+      <c r="A25" s="15">
         <v>43504</v>
       </c>
-      <c r="B25" s="14" t="s">
+      <c r="B25" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="C25" s="20">
+      <c r="C25" s="16">
         <v>7.2222222222222229E-2</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="19">
+      <c r="A26" s="15">
         <v>43505</v>
       </c>
-      <c r="B26" s="14" t="s">
+      <c r="B26" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="C26" s="20">
+      <c r="C26" s="16">
         <v>2.8472222222222222E-2</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="19">
+      <c r="A27" s="15">
         <v>43508</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="C27" s="20">
+      <c r="C27" s="16">
         <v>3.4722222222222224E-2</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="19">
+      <c r="A28" s="15">
         <v>43509</v>
       </c>
-      <c r="B28" s="14" t="s">
+      <c r="B28" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C28" s="20">
+      <c r="C28" s="16">
         <v>1.6666666666666666E-2</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="19">
+      <c r="A29" s="15">
         <v>43510</v>
       </c>
-      <c r="B29" s="14" t="s">
+      <c r="B29" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C29" s="20">
+      <c r="C29" s="16">
         <v>1.8055555555555557E-2</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" s="19">
+      <c r="A30" s="15">
         <v>43511</v>
       </c>
-      <c r="B30" s="14" t="s">
+      <c r="B30" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="C30" s="20">
+      <c r="C30" s="16">
         <v>2.5694444444444447E-2</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="19">
+      <c r="A31" s="15">
         <v>43514</v>
       </c>
-      <c r="B31" s="14" t="s">
+      <c r="B31" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C31" s="20">
+      <c r="C31" s="16">
         <v>4.3055555555555562E-2</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="19">
+      <c r="A32" s="15">
         <v>43517</v>
       </c>
-      <c r="B32" s="14" t="s">
+      <c r="B32" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="C32" s="20">
+      <c r="C32" s="16">
         <v>3.9583333333333331E-2</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A33" s="19">
+      <c r="A33" s="15">
         <v>43518</v>
       </c>
-      <c r="B33" s="14" t="s">
+      <c r="B33" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="C33" s="20">
+      <c r="C33" s="16">
         <v>2.2916666666666669E-2</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" s="19">
+      <c r="A34" s="15">
         <v>43519</v>
       </c>
-      <c r="B34" s="14" t="s">
+      <c r="B34" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="C34" s="20">
+      <c r="C34" s="16">
         <v>1.2499999999999999E-2</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" s="19">
+      <c r="A35" s="15">
         <v>43520</v>
       </c>
-      <c r="B35" s="14" t="s">
+      <c r="B35" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="C35" s="20">
+      <c r="C35" s="16">
         <v>3.7499999999999999E-2</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A36" s="19">
+      <c r="A36" s="15">
         <v>43526</v>
       </c>
-      <c r="B36" s="14" t="s">
+      <c r="B36" s="13" t="s">
         <v>68</v>
       </c>
-      <c r="C36" s="20">
+      <c r="C36" s="16">
         <v>6.7361111111111108E-2</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A37" s="19">
+      <c r="A37" s="15">
         <v>43527</v>
       </c>
-      <c r="B37" s="14" t="s">
+      <c r="B37" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="C37" s="20">
+      <c r="C37" s="16">
         <v>6.0416666666666667E-2</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A38" s="17"/>
-      <c r="B38" s="18" t="s">
+      <c r="A38" s="19"/>
+      <c r="B38" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C38" s="21">
+      <c r="C38" s="17">
         <f>SUM(C8:C37)</f>
         <v>1.3076388888888888</v>
       </c>

</xml_diff>